<commit_message>
obj model chart update
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="9540" windowHeight="9165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="9165"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>with obj</t>
+    <t>with obj &amp; visual-line</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -299,7 +299,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>with obj</c:v>
+                  <c:v>with obj &amp; visual-line</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -453,11 +453,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="374568736"/>
-        <c:axId val="374569296"/>
+        <c:axId val="372577168"/>
+        <c:axId val="372577728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="374568736"/>
+        <c:axId val="372577168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,7 +518,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374569296"/>
+        <c:crossAx val="372577728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -526,7 +526,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374569296"/>
+        <c:axId val="372577728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -642,7 +642,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374568736"/>
+        <c:crossAx val="372577168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -755,7 +755,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>with obj</c:v>
+                  <c:v>with obj &amp; visual-line</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1022,11 +1022,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="374572656"/>
-        <c:axId val="374573216"/>
+        <c:axId val="372581088"/>
+        <c:axId val="372581648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="374572656"/>
+        <c:axId val="372581088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1069,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374573216"/>
+        <c:crossAx val="372581648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1077,7 +1077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374573216"/>
+        <c:axId val="372581648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1192,7 +1192,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374572656"/>
+        <c:crossAx val="372581088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1296,6 +1296,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>with obj &amp; visual-line</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
@@ -1373,6 +1384,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$E$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$C$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
@@ -1390,6 +1408,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$E$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$C$2:$E$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1411,6 +1436,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no obj</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
@@ -1488,6 +1524,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$E$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$C$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
@@ -1505,6 +1548,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$3:$E$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$C$3:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1526,6 +1576,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no visual-line</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
@@ -1603,6 +1664,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$E$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$C$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
@@ -1620,6 +1688,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$4:$E$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$C$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1648,11 +1723,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="377915872"/>
-        <c:axId val="377916432"/>
+        <c:axId val="372585568"/>
+        <c:axId val="372586128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="377915872"/>
+        <c:axId val="372585568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1694,7 +1769,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377916432"/>
+        <c:crossAx val="372586128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1702,7 +1777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="377916432"/>
+        <c:axId val="372586128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,7 +1882,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377915872"/>
+        <c:crossAx val="372585568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1819,6 +1894,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3897,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="AC23" sqref="AC23"/>
+    <sheetView tabSelected="1" topLeftCell="I19" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>